<commit_message>
Restore to 19 countries
</commit_message>
<xml_diff>
--- a/Data/L3/fki.xlsx
+++ b/Data/L3/fki.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\MSc\Thesis\Data\L3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{73E600C7-61DE-4511-A168-3F3501D5D9A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555DEFC4-E670-407E-ACDB-721C47D405C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="28680" yWindow="-12375" windowWidth="18240" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fki" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>fki</t>
   </si>
@@ -74,12 +74,33 @@
   </si>
   <si>
     <t>IDN</t>
+  </si>
+  <si>
+    <t>NLD</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>BGR</t>
+  </si>
+  <si>
+    <t>LVA</t>
+  </si>
+  <si>
+    <t>RUS</t>
+  </si>
+  <si>
+    <t>SRB</t>
+  </si>
+  <si>
+    <t>CNT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -397,7 +418,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -512,6 +533,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -557,8 +598,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -913,290 +956,417 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C2">
-        <v>1.0289999999999999</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="E2">
-        <v>0.99</v>
+        <v>0.93899999999999995</v>
       </c>
       <c r="F2">
-        <v>0.59</v>
+        <v>0.64</v>
       </c>
       <c r="G2">
-        <v>1.4670000000000001</v>
+        <v>1.9670000000000001</v>
       </c>
       <c r="H2">
-        <v>1.58</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>0.81</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="E3">
-        <v>0.76700000000000002</v>
+        <v>0.99</v>
       </c>
       <c r="F3">
-        <v>0.60099999999999998</v>
+        <v>0.58899999999999997</v>
       </c>
       <c r="G3">
-        <v>1.603</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="H3">
-        <v>0.76700000000000002</v>
+        <v>1.407</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>0.66100000000000003</v>
+        <v>0.77100000000000002</v>
       </c>
       <c r="E4">
-        <v>0.73399999999999999</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="F4">
-        <v>0.46400000000000002</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="G4">
-        <v>1.012</v>
+        <v>1.145</v>
       </c>
       <c r="H4">
-        <v>0.67</v>
+        <v>0.80600000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>0.60899999999999999</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="E5">
-        <v>0.66400000000000003</v>
+        <v>0.85</v>
       </c>
       <c r="F5">
-        <v>0.63300000000000001</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="G5">
-        <v>0.32500000000000001</v>
+        <v>1.194</v>
       </c>
       <c r="H5">
-        <v>0.80100000000000005</v>
+        <v>0.56299999999999994</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>0.60599999999999998</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="E6">
-        <v>0.63900000000000001</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="F6">
-        <v>0.40100000000000002</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="G6">
-        <v>0.86899999999999999</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="H6">
-        <v>0.71899999999999997</v>
+        <v>0.72599999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>0.58899999999999997</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="E7">
-        <v>0.44900000000000001</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="F7">
-        <v>0.30199999999999999</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="G7">
-        <v>1.3720000000000001</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="H7">
-        <v>0.93899999999999995</v>
+        <v>0.83499999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>0.57599999999999996</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="E8">
-        <v>0.67200000000000004</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="F8">
-        <v>0.747</v>
+        <v>0.40100000000000002</v>
       </c>
       <c r="G8">
-        <v>0.41899999999999998</v>
+        <v>0.68</v>
       </c>
       <c r="H8">
-        <v>0.45500000000000002</v>
+        <v>0.76200000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>0.55200000000000005</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="E9">
-        <v>0.60799999999999998</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="F9">
-        <v>0.92400000000000004</v>
+        <v>0.76</v>
       </c>
       <c r="G9">
-        <v>0.41399999999999998</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="H9">
-        <v>0.34100000000000003</v>
+        <v>0.72799999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>0.54600000000000004</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="E10">
-        <v>0.59499999999999997</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="F10">
-        <v>0.7</v>
+        <v>0.747</v>
       </c>
       <c r="G10">
-        <v>0.35399999999999998</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="H10">
-        <v>0.503</v>
+        <v>0.57399999999999995</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>0.36899999999999999</v>
+        <v>0.56200000000000006</v>
       </c>
       <c r="E11">
-        <v>0.14099999999999999</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="F11">
-        <v>0.54800000000000004</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="G11">
-        <v>0.17399999999999999</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="H11">
-        <v>0.997</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>0.28899999999999998</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="E12">
-        <v>7.8E-2</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="F12">
-        <v>0.19400000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="G12">
-        <v>0.78</v>
+        <v>0.311</v>
       </c>
       <c r="H12">
-        <v>0.86799999999999999</v>
+        <v>0.57199999999999995</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>0.13100000000000001</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="E13">
-        <v>0.155</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="F13">
-        <v>0.01</v>
+        <v>0.30199999999999999</v>
       </c>
       <c r="G13">
-        <v>0.50600000000000001</v>
+        <v>0.81799999999999995</v>
       </c>
       <c r="H13">
-        <v>0.80900000000000005</v>
+        <v>0.90800000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="E14">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="F14">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="G14">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="H14">
+        <v>0.79400000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="E15">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="F15">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="G15">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="H15">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.249</v>
+      </c>
+      <c r="F16">
+        <v>0.5</v>
+      </c>
+      <c r="G16">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="H16">
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="E17">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="F17">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="G17">
+        <v>0.21</v>
+      </c>
+      <c r="H17">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>0.309</v>
+      </c>
+      <c r="E18">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="G18">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="H18">
+        <v>0.877</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.155</v>
+      </c>
+      <c r="F19">
+        <v>0.01</v>
+      </c>
+      <c r="G19">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="H19">
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14">
-        <v>0.104</v>
-      </c>
-      <c r="E14">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2">
+        <v>0.122</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2">
         <v>0.01</v>
       </c>
-      <c r="F14">
+      <c r="F20" s="2">
         <v>0.04</v>
       </c>
-      <c r="G14">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H14">
-        <v>0.73399999999999999</v>
+      <c r="G20" s="2">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.78700000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>